<commit_message>
Tue Feb 27 08:30:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary_2024-2/assess_绩效+软性考核表.xlsx
+++ b/lixiao/summary_2024-2/assess_绩效+软性考核表.xlsx
@@ -2183,17 +2183,17 @@
       </c>
       <c r="C7" s="23" t="inlineStr">
         <is>
-          <t>N2023121805</t>
+          <t>黎文华订单</t>
         </is>
       </c>
       <c r="D7" s="23" t="inlineStr">
         <is>
-          <t>其他业务</t>
+          <t/>
         </is>
       </c>
       <c r="E7" s="37" t="inlineStr">
         <is>
-          <t>无</t>
+          <t/>
         </is>
       </c>
       <c r="F7" s="23">
@@ -2201,105 +2201,345 @@
       </c>
       <c r="G7" s="38" t="inlineStr">
         <is>
+          <t>菌群+对应代谢产物介导+机制研究</t>
+        </is>
+      </c>
+      <c r="H7" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I7" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J7" s="48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K7" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B8" s="23">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="inlineStr">
+        <is>
+          <t>N2023121805</t>
+        </is>
+      </c>
+      <c r="D8" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E8" s="37" t="inlineStr">
+        <is>
+          <t>无</t>
+        </is>
+      </c>
+      <c r="F8" s="23">
+        <v>1</v>
+      </c>
+      <c r="G8" s="38" t="inlineStr">
+        <is>
           <t>网络药理学+Mandenol与piezo1分子对接</t>
         </is>
       </c>
-      <c r="H7" s="39" t="inlineStr">
+      <c r="H8" s="39" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="I7" s="23" t="inlineStr">
+      <c r="I8" s="23" t="inlineStr">
         <is>
           <t>完成</t>
         </is>
       </c>
-      <c r="J7" s="48" t="inlineStr">
+      <c r="J8" s="23" t="inlineStr">
         <is>
           <t>(1) 网络药理学; (2) 预测化合物靶点; (3) 获取疾病或条件相关的基因集:Genecards; (4) 疾病相关基因集:PharmGKB 数据库挖掘; (5) 疾病相关基因集:DisGeNet 数据库挖掘; (6) 调控该基因的相关转录因子 (TF) 数据获取; (7) 富集分析; (8) 全自动批量分子对接</t>
         </is>
       </c>
-      <c r="K7" s="23">
+      <c r="K8" s="23">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-    </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="23"/>
+      <c r="A9" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B9" s="23">
+        <v>3</v>
+      </c>
+      <c r="C9" s="23" t="inlineStr">
+        <is>
+          <t>BI2024013001</t>
+        </is>
+      </c>
+      <c r="D9" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E9" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F9" s="23">
+        <v>1</v>
+      </c>
+      <c r="G9" s="38" t="inlineStr">
+        <is>
+          <t>审核业务</t>
+        </is>
+      </c>
+      <c r="H9" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I9" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J9" s="48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K9" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="23"/>
+      <c r="A10" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B10" s="23">
+        <v>4</v>
+      </c>
+      <c r="C10" s="23" t="inlineStr">
+        <is>
+          <t>N2024020103</t>
+        </is>
+      </c>
+      <c r="D10" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E10" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F10" s="23">
+        <v>1</v>
+      </c>
+      <c r="G10" s="38" t="inlineStr">
+        <is>
+          <t>筛选主动脉-下腔静脉瘘ACF模型 DEGs 并功能分析</t>
+        </is>
+      </c>
+      <c r="H10" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I10" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J10" s="48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K10" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="A11" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B11" s="23">
+        <v>5</v>
+      </c>
+      <c r="C11" s="23" t="inlineStr">
+        <is>
+          <t>N2024012602</t>
+        </is>
+      </c>
+      <c r="D11" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E11" s="37" t="inlineStr">
+        <is>
+          <t>1.5-2分</t>
+        </is>
+      </c>
+      <c r="F11" s="23">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38" t="inlineStr">
+        <is>
+          <t>Hydroxysafflor Yellow A 与Piezo1对接</t>
+        </is>
+      </c>
+      <c r="H11" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I11" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J11" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K11" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="23"/>
+      <c r="A12" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B12" s="23">
+        <v>6</v>
+      </c>
+      <c r="C12" s="23" t="inlineStr">
+        <is>
+          <t>N2024010303</t>
+        </is>
+      </c>
+      <c r="D12" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E12" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F12" s="23">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38" t="inlineStr">
+        <is>
+          <t>分子对接 Celogenamide A（环状肽）蛋白 SSTR2</t>
+        </is>
+      </c>
+      <c r="H12" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I12" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J12" s="48" t="inlineStr">
+        <is>
+          <t>(1) 分子对接肽与蛋白</t>
+        </is>
+      </c>
+      <c r="K12" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="23"/>
+      <c r="A13" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B13" s="23">
+        <v>7</v>
+      </c>
+      <c r="C13" s="23" t="inlineStr">
+        <is>
+          <t>20231012</t>
+        </is>
+      </c>
+      <c r="D13" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E13" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F13" s="23">
+        <v>1</v>
+      </c>
+      <c r="G13" s="38" t="inlineStr">
+        <is>
+          <t>建立风险模型和作图</t>
+        </is>
+      </c>
+      <c r="H13" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I13" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J13" s="48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K13" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="23"/>
@@ -2483,23 +2723,23 @@
         <v>31</v>
       </c>
       <c r="F29" s="43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G29" s="26" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H29" s="26">
-        <v>0.1</v>
+      <c r="H29" s="26" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I29" s="51" t="inlineStr">
         <is>
-          <t>0.1=0.1</t>
-        </is>
-      </c>
-      <c r="J29" s="26">
-        <v>0.1</v>
+          <t>NA+0.1+NA+NA+NA+NA+NA=NA</t>
+        </is>
+      </c>
+      <c r="J29" s="26" t="e">
+        <v>#N/A</v>
       </c>
       <c r="K29" s="52"/>
     </row>

</xml_diff>

<commit_message>
Thu Feb 29 06:50:05 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary_2024-2/assess_绩效+软性考核表.xlsx
+++ b/lixiao/summary_2024-2/assess_绩效+软性考核表.xlsx
@@ -2071,7 +2071,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="C7" s="23" t="inlineStr">
         <is>
-          <t>黎文华订单</t>
+          <t>414731942</t>
         </is>
       </c>
       <c r="D7" s="23" t="inlineStr">
@@ -2219,10 +2219,26 @@
           <t/>
         </is>
       </c>
-      <c r="K7" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K7" s="23">
+        <v>0.142</v>
+      </c>
+      <c r="L7">
+        <v>852</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2275,6 +2291,34 @@
       <c r="K8" s="23">
         <v>0.1</v>
       </c>
+      <c r="L8">
+        <v>600</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="23" t="inlineStr">
@@ -2323,10 +2367,26 @@
           <t/>
         </is>
       </c>
-      <c r="K9" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K9" s="23">
+        <v>0.008</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2376,10 +2436,26 @@
           <t/>
         </is>
       </c>
-      <c r="K10" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K10" s="23">
+        <v>0.086</v>
+      </c>
+      <c r="L10">
+        <v>516</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2429,10 +2505,26 @@
           <t/>
         </is>
       </c>
-      <c r="K11" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K11" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="L11">
+        <v>180</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2479,13 +2571,29 @@
       </c>
       <c r="J12" s="48" t="inlineStr">
         <is>
-          <t>(1) 分子对接肽与蛋白</t>
-        </is>
-      </c>
-      <c r="K12" s="23" t="inlineStr">
-        <is>
           <t/>
         </is>
+      </c>
+      <c r="K12" s="23">
+        <v>0.086</v>
+      </c>
+      <c r="L12">
+        <v>516</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2535,37 +2643,165 @@
           <t/>
         </is>
       </c>
-      <c r="K13" s="23" t="inlineStr">
+      <c r="K13" s="23">
+        <v>0.086</v>
+      </c>
+      <c r="L13">
+        <v>516</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B14" s="23">
+        <v>8</v>
+      </c>
+      <c r="C14" s="23" t="inlineStr">
+        <is>
+          <t>20230815</t>
+        </is>
+      </c>
+      <c r="D14" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E14" s="37" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
+      <c r="F14" s="23">
+        <v>1</v>
+      </c>
+      <c r="G14" s="38" t="inlineStr">
+        <is>
+          <t>列线图模型建立与验证</t>
+        </is>
+      </c>
+      <c r="H14" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I14" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J14" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K14" s="23">
+        <v>0.058</v>
+      </c>
+      <c r="L14">
+        <v>348</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="23"/>
+      <c r="A15" s="23" t="inlineStr">
+        <is>
+          <t>黄礼闯</t>
+        </is>
+      </c>
+      <c r="B15" s="23">
+        <v>9</v>
+      </c>
+      <c r="C15" s="23" t="inlineStr">
+        <is>
+          <t>N2024022202</t>
+        </is>
+      </c>
+      <c r="D15" s="23" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="E15" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F15" s="23">
+        <v>1</v>
+      </c>
+      <c r="G15" s="38" t="inlineStr">
+        <is>
+          <t>乙肝病毒HBx利用泛素化系统降解XXX上调YYY诱导肝癌线粒体自噬</t>
+        </is>
+      </c>
+      <c r="H15" s="39" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I15" s="23" t="inlineStr">
+        <is>
+          <t>完成</t>
+        </is>
+      </c>
+      <c r="J15" s="48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="K15" s="23">
+        <v>0.114</v>
+      </c>
+      <c r="L15">
+        <v>684</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="23"/>
@@ -2723,23 +2959,23 @@
         <v>31</v>
       </c>
       <c r="F29" s="43">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G29" s="26" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H29" s="26" t="e">
-        <v>#N/A</v>
+      <c r="H29" s="26">
+        <v>0.71</v>
       </c>
       <c r="I29" s="51" t="inlineStr">
         <is>
-          <t>NA+0.1+NA+NA+NA+NA+NA=NA</t>
-        </is>
-      </c>
-      <c r="J29" s="26" t="e">
-        <v>#N/A</v>
+          <t>0.142+0.1+0.008+0.086+0.03+0.086+0.086+0.058+0.114=0.71</t>
+        </is>
+      </c>
+      <c r="J29" s="26">
+        <v>0.71</v>
       </c>
       <c r="K29" s="52"/>
     </row>

</xml_diff>